<commit_message>
[added] tested Project V2 with docs (V3 is the same)
</commit_message>
<xml_diff>
--- a/Project-v2(+ Forwarding)/Documents/2-operand/WITH_forw_no_haza/with_forw_no_haz_2_OP.xlsx
+++ b/Project-v2(+ Forwarding)/Documents/2-operand/WITH_forw_no_haza/with_forw_no_haz_2_OP.xlsx
@@ -200,10 +200,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -513,7 +513,7 @@
   <dimension ref="A1:AQ25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:F17"/>
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,11 +558,11 @@
       <c r="K2" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -588,11 +588,11 @@
       <c r="L3" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="Q3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="D4" s="4" t="s">
@@ -615,12 +615,12 @@
       <c r="M4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="S4" s="5" t="s">
+      <c r="S4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="D5" s="4" t="s">
@@ -643,13 +643,13 @@
       <c r="N5" t="s">
         <v>5</v>
       </c>
-      <c r="T5" s="5" t="s">
+      <c r="T5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -657,11 +657,11 @@
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
       <c r="K6" t="s">
         <v>1</v>
       </c>
@@ -680,13 +680,13 @@
       <c r="P6" t="s">
         <v>5</v>
       </c>
-      <c r="W6" s="5" t="s">
+      <c r="W6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="X6" s="5"/>
-      <c r="Y6" s="5"/>
-      <c r="Z6" s="5"/>
-      <c r="AA6" s="5"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -717,13 +717,13 @@
       <c r="Q7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="X7" s="5" t="s">
+      <c r="X7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="Y7" s="5"/>
-      <c r="Z7" s="5"/>
-      <c r="AA7" s="5"/>
-      <c r="AB7" s="5"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -754,14 +754,14 @@
       <c r="R8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Z8" s="5" t="s">
+      <c r="Z8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AA8" s="5"/>
-      <c r="AB8" s="5"/>
-      <c r="AC8" s="5"/>
-      <c r="AD8" s="5"/>
-      <c r="AE8" s="5"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -769,11 +769,11 @@
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
       <c r="N9" t="s">
         <v>1</v>
       </c>
@@ -792,14 +792,14 @@
       <c r="S9" t="s">
         <v>5</v>
       </c>
-      <c r="AB9" s="5" t="s">
+      <c r="AB9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="AC9" s="5"/>
-      <c r="AD9" s="5"/>
-      <c r="AE9" s="5"/>
-      <c r="AF9" s="5"/>
-      <c r="AG9" s="5"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="6"/>
+      <c r="AE9" s="6"/>
+      <c r="AF9" s="6"/>
+      <c r="AG9" s="6"/>
     </row>
     <row r="10" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -830,14 +830,14 @@
       <c r="T10" t="s">
         <v>5</v>
       </c>
-      <c r="AD10" s="5" t="s">
+      <c r="AD10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="AE10" s="5"/>
-      <c r="AF10" s="5"/>
-      <c r="AG10" s="5"/>
-      <c r="AH10" s="5"/>
-      <c r="AI10" s="5"/>
+      <c r="AE10" s="6"/>
+      <c r="AF10" s="6"/>
+      <c r="AG10" s="6"/>
+      <c r="AH10" s="6"/>
+      <c r="AI10" s="6"/>
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -871,14 +871,14 @@
       <c r="V11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AF11" s="5" t="s">
+      <c r="AF11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AG11" s="5"/>
-      <c r="AH11" s="5"/>
-      <c r="AI11" s="5"/>
-      <c r="AJ11" s="5"/>
-      <c r="AK11" s="5"/>
+      <c r="AG11" s="6"/>
+      <c r="AH11" s="6"/>
+      <c r="AI11" s="6"/>
+      <c r="AJ11" s="6"/>
+      <c r="AK11" s="6"/>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -886,11 +886,11 @@
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
       <c r="Q12" t="s">
         <v>1</v>
       </c>
@@ -915,14 +915,14 @@
       <c r="X12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AH12" s="5" t="s">
+      <c r="AH12" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AI12" s="5"/>
-      <c r="AJ12" s="5"/>
-      <c r="AK12" s="5"/>
-      <c r="AL12" s="5"/>
-      <c r="AM12" s="5"/>
+      <c r="AI12" s="6"/>
+      <c r="AJ12" s="6"/>
+      <c r="AK12" s="6"/>
+      <c r="AL12" s="6"/>
+      <c r="AM12" s="6"/>
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -930,11 +930,11 @@
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
       <c r="R13" t="s">
         <v>1</v>
       </c>
@@ -959,16 +959,16 @@
       <c r="Y13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AJ13" s="5" t="s">
+      <c r="AJ13" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="AK13" s="5"/>
-      <c r="AL13" s="5"/>
-      <c r="AM13" s="5"/>
-      <c r="AN13" s="5"/>
-      <c r="AO13" s="5"/>
-      <c r="AP13" s="5"/>
-      <c r="AQ13" s="5"/>
+      <c r="AK13" s="6"/>
+      <c r="AL13" s="6"/>
+      <c r="AM13" s="6"/>
+      <c r="AN13" s="6"/>
+      <c r="AO13" s="6"/>
+      <c r="AP13" s="6"/>
+      <c r="AQ13" s="6"/>
     </row>
     <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -976,11 +976,11 @@
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
       <c r="S14" t="s">
         <v>1</v>
       </c>
@@ -1005,28 +1005,28 @@
       <c r="Z14" t="s">
         <v>5</v>
       </c>
-      <c r="AL14" s="5" t="s">
+      <c r="AL14" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="AM14" s="5"/>
-      <c r="AN14" s="5"/>
-      <c r="AO14" s="5"/>
-      <c r="AP14" s="5"/>
-      <c r="AQ14" s="5"/>
+      <c r="AM14" s="6"/>
+      <c r="AN14" s="6"/>
+      <c r="AO14" s="6"/>
+      <c r="AP14" s="6"/>
+      <c r="AQ14" s="6"/>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C19" s="3"/>
@@ -1048,31 +1048,11 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="S4:V4"/>
-    <mergeCell ref="T5:X5"/>
-    <mergeCell ref="W6:AA6"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="X7:AB7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="Z8:AE8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="AB9:AG9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="AD10:AI10"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="A13:C13"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="AL14:AQ14"/>
@@ -1083,11 +1063,31 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="AH12:AM12"/>
     <mergeCell ref="AJ13:AQ13"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="AB9:AG9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="AD10:AI10"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="X7:AB7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="Z8:AE8"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="S4:V4"/>
+    <mergeCell ref="T5:X5"/>
+    <mergeCell ref="W6:AA6"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>